<commit_message>
Used back original food list and updated code
</commit_message>
<xml_diff>
--- a/original_food_list.xlsx
+++ b/original_food_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\PycharmProjects\AI_ChatBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0195E41B-3F6E-475D-B7E3-42736A37467D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA424D2E-A10D-4C16-8199-80C0E1499AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,12 +198,6 @@
     <t>Korean</t>
   </si>
   <si>
-    <t xml:space="preserve">Tteok </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kimchi </t>
-  </si>
-  <si>
     <t>Gimbap</t>
   </si>
   <si>
@@ -319,6 +313,12 @@
   </si>
   <si>
     <t>Vegetarian Dinner Set (Chawanmushi)</t>
+  </si>
+  <si>
+    <t>Tteok</t>
+  </si>
+  <si>
+    <t>Kimchi</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1266,7 +1268,7 @@
         <v>56</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="C49" s="2">
         <v>2</v>
@@ -1280,7 +1282,7 @@
         <v>56</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="C50" s="2">
         <v>4</v>
@@ -1294,7 +1296,7 @@
         <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C51" s="2">
         <v>4.5</v>
@@ -1308,7 +1310,7 @@
         <v>56</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C52" s="2">
         <v>5</v>
@@ -1322,7 +1324,7 @@
         <v>56</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C53" s="2">
         <v>6</v>
@@ -1336,7 +1338,7 @@
         <v>56</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C54" s="2">
         <v>6.5</v>
@@ -1350,7 +1352,7 @@
         <v>56</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C55" s="2">
         <v>7</v>
@@ -1364,7 +1366,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C56" s="2">
         <v>7</v>
@@ -1378,7 +1380,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C57" s="2">
         <v>7</v>
@@ -1392,7 +1394,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C58" s="2">
         <v>7.5</v>
@@ -1406,7 +1408,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C59" s="2">
         <v>8</v>
@@ -1420,7 +1422,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C60" s="2">
         <v>8</v>
@@ -1434,7 +1436,7 @@
         <v>56</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C61" s="2">
         <v>8.5</v>
@@ -1448,7 +1450,7 @@
         <v>56</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C62" s="2">
         <v>9</v>
@@ -1462,7 +1464,7 @@
         <v>56</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C63" s="2">
         <v>10</v>
@@ -1473,10 +1475,10 @@
     </row>
     <row r="64" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C64" s="2">
         <v>1.5</v>
@@ -1487,10 +1489,10 @@
     </row>
     <row r="65" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C65" s="2">
         <v>1.5</v>
@@ -1501,10 +1503,10 @@
     </row>
     <row r="66" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C66" s="2">
         <v>5</v>
@@ -1515,10 +1517,10 @@
     </row>
     <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C67" s="2">
         <v>5</v>
@@ -1529,10 +1531,10 @@
     </row>
     <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C68" s="2">
         <v>1.5</v>
@@ -1543,10 +1545,10 @@
     </row>
     <row r="69" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C69" s="2">
         <v>8</v>
@@ -1557,10 +1559,10 @@
     </row>
     <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C70" s="2">
         <v>6.5</v>
@@ -1571,10 +1573,10 @@
     </row>
     <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C71" s="2">
         <v>9</v>
@@ -1585,10 +1587,10 @@
     </row>
     <row r="72" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C72" s="2">
         <v>8</v>
@@ -1599,10 +1601,10 @@
     </row>
     <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C73" s="2">
         <v>7</v>
@@ -1613,10 +1615,10 @@
     </row>
     <row r="74" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C74" s="2">
         <v>7</v>
@@ -1627,10 +1629,10 @@
     </row>
     <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C75" s="2">
         <v>6</v>
@@ -1641,10 +1643,10 @@
     </row>
     <row r="76" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C76" s="2">
         <v>6</v>
@@ -1655,10 +1657,10 @@
     </row>
     <row r="77" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C77" s="2">
         <v>7</v>
@@ -1669,10 +1671,10 @@
     </row>
     <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C78" s="2">
         <v>7</v>
@@ -1683,10 +1685,10 @@
     </row>
     <row r="79" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C79" s="2">
         <v>7</v>
@@ -1697,10 +1699,10 @@
     </row>
     <row r="80" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C80" s="2">
         <v>6</v>
@@ -1711,10 +1713,10 @@
     </row>
     <row r="81" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C81" s="2">
         <v>6</v>
@@ -1725,10 +1727,10 @@
     </row>
     <row r="82" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C82" s="2">
         <v>7</v>
@@ -1739,10 +1741,10 @@
     </row>
     <row r="83" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C83" s="2">
         <v>10</v>
@@ -1753,10 +1755,10 @@
     </row>
     <row r="84" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C84" s="2">
         <v>9</v>
@@ -1767,10 +1769,10 @@
     </row>
     <row r="85" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C85" s="2">
         <v>8</v>
@@ -1781,10 +1783,10 @@
     </row>
     <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C86" s="2">
         <v>10</v>
@@ -1795,10 +1797,10 @@
     </row>
     <row r="87" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C87" s="2">
         <v>9</v>
@@ -1809,10 +1811,10 @@
     </row>
     <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C88" s="2">
         <v>8</v>

</xml_diff>